<commit_message>
multiple pies working, need object and color constancy
</commit_message>
<xml_diff>
--- a/Excel sketches.xlsx
+++ b/Excel sketches.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <r>
       <t>time10to14</t>
@@ -255,6 +255,57 @@
   </si>
   <si>
     <t>carpool</t>
+  </si>
+  <si>
+    <t>16000US2507000</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>geoid</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>population</t>
+  </si>
+  <si>
+    <t>totalCommute</t>
+  </si>
+  <si>
+    <t>overallAverageTime</t>
+  </si>
+  <si>
+    <t>droveCar</t>
+  </si>
+  <si>
+    <t>droveAlone</t>
+  </si>
+  <si>
+    <t>carpool2Person</t>
+  </si>
+  <si>
+    <t>carpool3Person</t>
+  </si>
+  <si>
+    <t>publicTransit</t>
+  </si>
+  <si>
+    <t>Bus</t>
+  </si>
+  <si>
+    <t>streetCar</t>
+  </si>
+  <si>
+    <t>railFerry</t>
+  </si>
+  <si>
+    <t>walked</t>
+  </si>
+  <si>
+    <t>taxi</t>
   </si>
 </sst>
 </file>
@@ -308,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -316,6 +367,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,11 +656,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="60578432"/>
-        <c:axId val="60576896"/>
+        <c:axId val="58350976"/>
+        <c:axId val="65689088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="60578432"/>
+        <c:axId val="58350976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -618,12 +670,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60576896"/>
+        <c:crossAx val="65689088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60576896"/>
+        <c:axId val="65689088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -634,7 +686,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60578432"/>
+        <c:crossAx val="58350976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -978,13 +1030,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
@@ -1167,20 +1222,208 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" t="s">
+        <v>24</v>
+      </c>
+      <c r="L23" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" t="s">
+        <v>26</v>
+      </c>
+      <c r="N23" t="s">
+        <v>27</v>
+      </c>
+      <c r="O23" t="s">
+        <v>28</v>
+      </c>
+      <c r="P23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="3">
+        <v>644710</v>
+      </c>
+      <c r="D24">
+        <v>310740</v>
+      </c>
+      <c r="E24">
+        <v>29.6</v>
+      </c>
+      <c r="F24">
+        <v>145967</v>
+      </c>
+      <c r="G24">
+        <v>123510</v>
+      </c>
+      <c r="H24">
+        <v>22457</v>
+      </c>
+      <c r="I24">
+        <v>17069</v>
+      </c>
+      <c r="J24">
+        <v>5388</v>
+      </c>
+      <c r="K24">
+        <v>107375</v>
+      </c>
+      <c r="L24">
+        <v>42442</v>
+      </c>
+      <c r="M24">
+        <v>60942</v>
+      </c>
+      <c r="N24">
+        <v>3991</v>
+      </c>
+      <c r="O24">
+        <v>48911</v>
+      </c>
+      <c r="P24">
+        <v>8487</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D25" s="3">
+        <v>10047830</v>
+      </c>
+      <c r="F25" s="3">
+        <v>4407145</v>
+      </c>
+      <c r="G25" s="3">
+        <v>3838050</v>
+      </c>
+      <c r="H25" s="3">
+        <v>569095</v>
+      </c>
+      <c r="I25" s="3">
+        <v>360675</v>
+      </c>
+      <c r="J25" s="3">
+        <v>208420</v>
+      </c>
+      <c r="K25" s="3">
+        <v>4561810</v>
+      </c>
+      <c r="L25" s="3">
+        <v>2075490</v>
+      </c>
+      <c r="M25" s="3">
+        <v>2324405</v>
+      </c>
+      <c r="N25" s="3">
+        <v>161915</v>
+      </c>
+      <c r="O25" s="3">
+        <v>744870</v>
+      </c>
+      <c r="P25" s="3">
+        <v>334005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <f>D25/D24</f>
+        <v>32.335167664285251</v>
+      </c>
+      <c r="F26">
+        <f t="shared" ref="E26:M26" si="0">F25/F24</f>
+        <v>30.192749046017251</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>31.074811756133105</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>25.341541612860134</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>21.130411857753824</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>38.682256867112102</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>42.484842840512222</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>48.901795391357616</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="0"/>
+        <v>38.141265465524597</v>
+      </c>
+      <c r="N26">
+        <f>N25/N24</f>
+        <v>40.5700325732899</v>
+      </c>
+      <c r="O26">
+        <f t="shared" ref="O26" si="1">O25/O24</f>
+        <v>15.229089570853182</v>
+      </c>
+      <c r="P26">
+        <f t="shared" ref="P26" si="2">P25/P24</f>
+        <v>39.354895722870275</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>